<commit_message>
40 runs xlsx + png
</commit_message>
<xml_diff>
--- a/final_demo/safety_with_fear_end_times.xlsx
+++ b/final_demo/safety_with_fear_end_times.xlsx
@@ -377,7 +377,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -631,6 +631,86 @@
         <v>102</v>
       </c>
     </row>
+    <row r="32" spans="1:2">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>100.8333333333333</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>83.93333333333334</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>149.7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>91.90000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>101.4833333333333</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>42.81666666666667</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>45.48333333333333</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39">
+        <v>37.53333333333333</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40">
+        <v>42.76666666666667</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <v>117.6166666666667</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>